<commit_message>
update water isotope data with ALHIC2302 158 L
</commit_message>
<xml_diff>
--- a/data/sampling/water_iso/water_iso_depths.xlsx
+++ b/data/sampling/water_iso/water_iso_depths.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1060" yWindow="760" windowWidth="29200" windowHeight="18880" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1060" yWindow="760" windowWidth="14120" windowHeight="18880" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sample_thicknesses" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="3">
+  <fonts count="4">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -32,6 +32,11 @@
       <color rgb="FF000000"/>
       <sz val="12"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <b val="1"/>
+      <sz val="12"/>
     </font>
     <font>
       <b val="1"/>
@@ -51,12 +56,27 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -69,11 +89,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -478,7 +501,7 @@
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="topRight" activeCell="I1" sqref="I1"/>
+      <selection pane="topRight" activeCell="C49" sqref="C49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="16"/>
@@ -2084,7 +2107,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+      <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2281,7 +2304,7 @@
         <v>127.68</v>
       </c>
       <c r="D6" t="n">
-        <v>0</v>
+        <v>35</v>
       </c>
       <c r="E6" t="n">
         <v>0</v>
@@ -2314,7 +2337,7 @@
         <v>127.68</v>
       </c>
       <c r="D7" t="n">
-        <v>35</v>
+        <v>0</v>
       </c>
       <c r="E7" t="n">
         <v>94</v>
@@ -2323,10 +2346,10 @@
         <v>74</v>
       </c>
       <c r="G7" s="2" t="n">
-        <v>70</v>
+        <v>81</v>
       </c>
       <c r="H7" s="2" t="n">
-        <v>90</v>
+        <v>66</v>
       </c>
       <c r="I7" t="inlineStr">
         <is>
@@ -2486,109 +2509,109 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="3" t="inlineStr">
+      <c r="B1" s="4" t="inlineStr">
         <is>
           <t>alhic1901-230_4-l_td</t>
         </is>
       </c>
-      <c r="C1" s="3" t="inlineStr">
+      <c r="C1" s="4" t="inlineStr">
         <is>
           <t>alhic1901-230_4-l_bd</t>
         </is>
       </c>
-      <c r="D1" s="3" t="inlineStr">
+      <c r="D1" s="4" t="inlineStr">
         <is>
           <t>alhic1901-230_4-r_td</t>
         </is>
       </c>
-      <c r="E1" s="3" t="inlineStr">
+      <c r="E1" s="4" t="inlineStr">
         <is>
           <t>alhic1901-230_4-r_bd</t>
         </is>
       </c>
-      <c r="F1" s="3" t="inlineStr">
+      <c r="F1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-155_2-l_td</t>
         </is>
       </c>
-      <c r="G1" s="3" t="inlineStr">
+      <c r="G1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-155_2-l_bd</t>
         </is>
       </c>
-      <c r="H1" s="3" t="inlineStr">
+      <c r="H1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-155_2-r_td</t>
         </is>
       </c>
-      <c r="I1" s="3" t="inlineStr">
+      <c r="I1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-155_2-r_bd</t>
         </is>
       </c>
-      <c r="J1" s="3" t="inlineStr">
+      <c r="J1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-156_2-l_td</t>
         </is>
       </c>
-      <c r="K1" s="3" t="inlineStr">
+      <c r="K1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-156_2-l_bd</t>
         </is>
       </c>
-      <c r="L1" s="3" t="inlineStr">
+      <c r="L1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-156_2-r_td</t>
         </is>
       </c>
-      <c r="M1" s="3" t="inlineStr">
+      <c r="M1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-156_2-r_bd</t>
         </is>
       </c>
-      <c r="N1" s="3" t="inlineStr">
+      <c r="N1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-158-l_td</t>
         </is>
       </c>
-      <c r="O1" s="3" t="inlineStr">
+      <c r="O1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-158-l_bd</t>
         </is>
       </c>
-      <c r="P1" s="3" t="inlineStr">
+      <c r="P1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-158-r_td</t>
         </is>
       </c>
-      <c r="Q1" s="3" t="inlineStr">
+      <c r="Q1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-158-r_bd</t>
         </is>
       </c>
-      <c r="R1" s="3" t="inlineStr">
+      <c r="R1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-159_3-l_td</t>
         </is>
       </c>
-      <c r="S1" s="3" t="inlineStr">
+      <c r="S1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-159_3-l_bd</t>
         </is>
       </c>
-      <c r="T1" s="3" t="inlineStr">
+      <c r="T1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-159_3-r_td</t>
         </is>
       </c>
-      <c r="U1" s="3" t="inlineStr">
+      <c r="U1" s="4" t="inlineStr">
         <is>
           <t>alhic2302-159_3-r_bd</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="n">
+      <c r="A2" s="4" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -2616,16 +2639,16 @@
         <v>126.404</v>
       </c>
       <c r="J2" t="n">
+        <v>127.715</v>
+      </c>
+      <c r="K2" t="n">
+        <v>127.725</v>
+      </c>
+      <c r="L2" t="n">
         <v>127.68</v>
       </c>
-      <c r="K2" t="n">
-        <v>127.69</v>
-      </c>
-      <c r="L2" t="n">
-        <v>127.715</v>
-      </c>
       <c r="M2" t="n">
-        <v>127.729</v>
+        <v>127.694</v>
       </c>
       <c r="N2" t="n">
         <v>128.696</v>
@@ -2653,7 +2676,7 @@
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="3" t="n">
+      <c r="A3" s="4" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
@@ -2681,16 +2704,16 @@
         <v>126.415</v>
       </c>
       <c r="J3" t="n">
-        <v>127.69</v>
+        <v>127.725</v>
       </c>
       <c r="K3" t="n">
-        <v>127.701</v>
+        <v>127.736</v>
       </c>
       <c r="L3" t="n">
-        <v>127.729</v>
+        <v>127.694</v>
       </c>
       <c r="M3" t="n">
-        <v>127.744</v>
+        <v>127.709</v>
       </c>
       <c r="N3" t="n">
         <v>128.708</v>
@@ -2718,7 +2741,7 @@
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="3" t="n">
+      <c r="A4" s="4" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
@@ -2746,16 +2769,16 @@
         <v>126.426</v>
       </c>
       <c r="J4" t="n">
-        <v>127.701</v>
+        <v>127.736</v>
       </c>
       <c r="K4" t="n">
-        <v>127.712</v>
+        <v>127.747</v>
       </c>
       <c r="L4" t="n">
-        <v>127.744</v>
+        <v>127.709</v>
       </c>
       <c r="M4" t="n">
-        <v>127.759</v>
+        <v>127.724</v>
       </c>
       <c r="N4" t="n">
         <v>128.721</v>
@@ -2783,7 +2806,7 @@
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="3" t="n">
+      <c r="A5" s="4" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="n">
@@ -2811,16 +2834,16 @@
         <v>126.439</v>
       </c>
       <c r="J5" t="n">
-        <v>127.712</v>
+        <v>127.747</v>
       </c>
       <c r="K5" t="n">
+        <v>127.759</v>
+      </c>
+      <c r="L5" t="n">
         <v>127.724</v>
       </c>
-      <c r="L5" t="n">
-        <v>127.759</v>
-      </c>
       <c r="M5" t="n">
-        <v>127.774</v>
+        <v>127.739</v>
       </c>
       <c r="N5" t="n">
         <v>128.734</v>
@@ -2848,7 +2871,7 @@
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="3" t="n">
+      <c r="A6" s="4" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="n">
@@ -2876,16 +2899,16 @@
         <v>126.453</v>
       </c>
       <c r="J6" t="n">
-        <v>127.724</v>
+        <v>127.759</v>
       </c>
       <c r="K6" t="n">
-        <v>127.735</v>
+        <v>127.77</v>
       </c>
       <c r="L6" t="n">
-        <v>127.774</v>
+        <v>127.739</v>
       </c>
       <c r="M6" t="n">
-        <v>127.789</v>
+        <v>127.754</v>
       </c>
       <c r="N6" t="n">
         <v>128.747</v>
@@ -2913,7 +2936,7 @@
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="3" t="n">
+      <c r="A7" s="4" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="n">
@@ -2941,16 +2964,16 @@
         <v>126.466</v>
       </c>
       <c r="J7" t="n">
-        <v>127.735</v>
+        <v>127.77</v>
       </c>
       <c r="K7" t="n">
-        <v>127.746</v>
+        <v>127.781</v>
       </c>
       <c r="L7" t="n">
-        <v>127.789</v>
+        <v>127.754</v>
       </c>
       <c r="M7" t="n">
-        <v>127.804</v>
+        <v>127.769</v>
       </c>
       <c r="N7" t="n">
         <v>128.76</v>
@@ -2978,7 +3001,7 @@
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="3" t="n">
+      <c r="A8" s="4" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="n">
@@ -3006,16 +3029,16 @@
         <v>126.479</v>
       </c>
       <c r="J8" t="n">
-        <v>127.746</v>
+        <v>127.781</v>
       </c>
       <c r="K8" t="n">
-        <v>127.757</v>
+        <v>127.792</v>
       </c>
       <c r="L8" t="n">
-        <v>127.804</v>
+        <v>127.769</v>
       </c>
       <c r="M8" t="n">
-        <v>127.819</v>
+        <v>127.784</v>
       </c>
       <c r="N8" t="n">
         <v>128.773</v>
@@ -3043,7 +3066,7 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="3" t="n">
+      <c r="A9" s="4" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="n">
@@ -3071,16 +3094,16 @@
         <v>126.492</v>
       </c>
       <c r="J9" t="n">
-        <v>127.757</v>
+        <v>127.792</v>
       </c>
       <c r="K9" t="n">
-        <v>127.768</v>
+        <v>127.804</v>
       </c>
       <c r="L9" t="n">
-        <v>127.819</v>
+        <v>127.784</v>
       </c>
       <c r="M9" t="n">
-        <v>127.834</v>
+        <v>127.799</v>
       </c>
       <c r="N9" t="n">
         <v>128.786</v>
@@ -3108,7 +3131,7 @@
       </c>
     </row>
     <row r="10">
-      <c r="A10" s="3" t="n">
+      <c r="A10" s="4" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="n">
@@ -3136,16 +3159,16 @@
         <v>126.505</v>
       </c>
       <c r="J10" t="n">
-        <v>127.768</v>
+        <v>127.804</v>
       </c>
       <c r="K10" t="n">
-        <v>127.78</v>
+        <v>127.815</v>
       </c>
       <c r="L10" t="n">
-        <v>127.834</v>
+        <v>127.799</v>
       </c>
       <c r="M10" t="n">
-        <v>127.849</v>
+        <v>127.814</v>
       </c>
       <c r="N10" t="n">
         <v>128.799</v>
@@ -3173,7 +3196,7 @@
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="3" t="n">
+      <c r="A11" s="4" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="n">
@@ -3201,16 +3224,16 @@
         <v>126.518</v>
       </c>
       <c r="J11" t="n">
-        <v>127.78</v>
+        <v>127.815</v>
       </c>
       <c r="K11" t="n">
-        <v>127.791</v>
+        <v>127.826</v>
       </c>
       <c r="L11" t="n">
-        <v>127.849</v>
+        <v>127.814</v>
       </c>
       <c r="M11" t="n">
-        <v>127.864</v>
+        <v>127.829</v>
       </c>
       <c r="N11" t="n">
         <v>128.812</v>
@@ -3238,7 +3261,7 @@
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="3" t="n">
+      <c r="A12" s="4" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="n">
@@ -3266,16 +3289,16 @@
         <v>126.532</v>
       </c>
       <c r="J12" t="n">
-        <v>127.791</v>
+        <v>127.826</v>
       </c>
       <c r="K12" t="n">
-        <v>127.802</v>
+        <v>127.837</v>
       </c>
       <c r="L12" t="n">
-        <v>127.864</v>
+        <v>127.829</v>
       </c>
       <c r="M12" t="n">
-        <v>127.879</v>
+        <v>127.844</v>
       </c>
       <c r="N12" t="n">
         <v>128.825</v>
@@ -3303,7 +3326,7 @@
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="3" t="n">
+      <c r="A13" s="4" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="n">
@@ -3331,16 +3354,16 @@
         <v>126.545</v>
       </c>
       <c r="J13" t="n">
-        <v>127.802</v>
+        <v>127.837</v>
       </c>
       <c r="K13" t="n">
-        <v>127.813</v>
+        <v>127.848</v>
       </c>
       <c r="L13" t="n">
-        <v>127.879</v>
+        <v>127.844</v>
       </c>
       <c r="M13" t="n">
-        <v>127.895</v>
+        <v>127.86</v>
       </c>
       <c r="N13" t="n">
         <v>128.838</v>
@@ -3368,7 +3391,7 @@
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="3" t="n">
+      <c r="A14" s="4" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="n">
@@ -3396,16 +3419,16 @@
         <v>126.558</v>
       </c>
       <c r="J14" t="n">
-        <v>127.813</v>
+        <v>127.848</v>
       </c>
       <c r="K14" t="n">
-        <v>127.825</v>
+        <v>127.86</v>
       </c>
       <c r="L14" t="n">
-        <v>127.895</v>
+        <v>127.86</v>
       </c>
       <c r="M14" t="n">
-        <v>127.91</v>
+        <v>127.875</v>
       </c>
       <c r="N14" t="n">
         <v>128.851</v>
@@ -3433,7 +3456,7 @@
       </c>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="n">
+      <c r="A15" s="4" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="n">
@@ -3461,16 +3484,16 @@
         <v>126.571</v>
       </c>
       <c r="J15" t="n">
-        <v>127.825</v>
+        <v>127.86</v>
       </c>
       <c r="K15" t="n">
-        <v>127.836</v>
+        <v>127.871</v>
       </c>
       <c r="L15" t="n">
-        <v>127.91</v>
+        <v>127.875</v>
       </c>
       <c r="M15" t="n">
-        <v>127.925</v>
+        <v>127.89</v>
       </c>
       <c r="N15" t="n">
         <v>128.864</v>
@@ -3498,7 +3521,7 @@
       </c>
     </row>
     <row r="16">
-      <c r="A16" s="3" t="n">
+      <c r="A16" s="4" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="n">
@@ -3526,16 +3549,16 @@
         <v>126.584</v>
       </c>
       <c r="J16" t="n">
-        <v>127.836</v>
+        <v>127.871</v>
       </c>
       <c r="K16" t="n">
-        <v>127.847</v>
+        <v>127.882</v>
       </c>
       <c r="L16" t="n">
-        <v>127.925</v>
+        <v>127.89</v>
       </c>
       <c r="M16" t="n">
-        <v>127.94</v>
+        <v>127.905</v>
       </c>
       <c r="N16" t="n">
         <v>128.877</v>
@@ -3563,7 +3586,7 @@
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="3" t="n">
+      <c r="A17" s="4" t="n">
         <v>15</v>
       </c>
       <c r="B17" t="n">
@@ -3591,16 +3614,16 @@
         <v>126.597</v>
       </c>
       <c r="J17" t="n">
-        <v>127.847</v>
+        <v>127.882</v>
       </c>
       <c r="K17" t="n">
-        <v>127.858</v>
+        <v>127.893</v>
       </c>
       <c r="L17" t="n">
-        <v>127.94</v>
+        <v>127.905</v>
       </c>
       <c r="M17" t="n">
-        <v>127.955</v>
+        <v>127.92</v>
       </c>
       <c r="N17" t="n">
         <v>128.89</v>
@@ -3628,7 +3651,7 @@
       </c>
     </row>
     <row r="18">
-      <c r="A18" s="3" t="n">
+      <c r="A18" s="4" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="n">
@@ -3656,16 +3679,16 @@
         <v>126.61</v>
       </c>
       <c r="J18" t="n">
-        <v>127.858</v>
+        <v>127.893</v>
       </c>
       <c r="K18" t="n">
-        <v>127.869</v>
+        <v>127.904</v>
       </c>
       <c r="L18" t="n">
-        <v>127.955</v>
+        <v>127.92</v>
       </c>
       <c r="M18" t="n">
-        <v>127.97</v>
+        <v>127.935</v>
       </c>
       <c r="N18" t="n">
         <v>128.903</v>
@@ -3693,7 +3716,7 @@
       </c>
     </row>
     <row r="19">
-      <c r="A19" s="3" t="n">
+      <c r="A19" s="4" t="n">
         <v>17</v>
       </c>
       <c r="B19" t="n">
@@ -3721,16 +3744,16 @@
         <v>126.624</v>
       </c>
       <c r="J19" t="n">
-        <v>127.869</v>
+        <v>127.904</v>
       </c>
       <c r="K19" t="n">
-        <v>127.881</v>
+        <v>127.916</v>
       </c>
       <c r="L19" t="n">
-        <v>127.97</v>
+        <v>127.935</v>
       </c>
       <c r="M19" t="n">
-        <v>127.985</v>
+        <v>127.95</v>
       </c>
       <c r="N19" t="n">
         <v>128.916</v>
@@ -3758,7 +3781,7 @@
       </c>
     </row>
     <row r="20">
-      <c r="A20" s="3" t="n">
+      <c r="A20" s="4" t="n">
         <v>18</v>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -3782,16 +3805,16 @@
         <v>126.637</v>
       </c>
       <c r="J20" t="n">
-        <v>127.881</v>
+        <v>127.916</v>
       </c>
       <c r="K20" t="n">
-        <v>127.892</v>
+        <v>127.927</v>
       </c>
       <c r="L20" t="n">
-        <v>127.985</v>
+        <v>127.95</v>
       </c>
       <c r="M20" t="n">
-        <v>128</v>
+        <v>127.965</v>
       </c>
       <c r="N20" t="n">
         <v>128.929</v>
@@ -3819,7 +3842,7 @@
       </c>
     </row>
     <row r="21">
-      <c r="A21" s="3" t="n">
+      <c r="A21" s="4" t="n">
         <v>19</v>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -3839,16 +3862,16 @@
         <v>126.65</v>
       </c>
       <c r="J21" t="n">
-        <v>127.892</v>
+        <v>127.927</v>
       </c>
       <c r="K21" t="n">
-        <v>127.903</v>
+        <v>127.938</v>
       </c>
       <c r="L21" t="n">
-        <v>128</v>
+        <v>127.965</v>
       </c>
       <c r="M21" t="n">
-        <v>128.015</v>
+        <v>127.98</v>
       </c>
       <c r="N21" t="n">
         <v>128.942</v>
@@ -3876,7 +3899,7 @@
       </c>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="n">
+      <c r="A22" s="4" t="n">
         <v>20</v>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -3896,16 +3919,16 @@
         <v>126.663</v>
       </c>
       <c r="J22" t="n">
-        <v>127.903</v>
+        <v>127.938</v>
       </c>
       <c r="K22" t="n">
-        <v>127.914</v>
+        <v>127.949</v>
       </c>
       <c r="L22" t="n">
-        <v>128.015</v>
+        <v>127.98</v>
       </c>
       <c r="M22" t="n">
-        <v>128.03</v>
+        <v>127.995</v>
       </c>
       <c r="N22" t="n">
         <v>128.955</v>
@@ -3933,7 +3956,7 @@
       </c>
     </row>
     <row r="23">
-      <c r="A23" s="3" t="n">
+      <c r="A23" s="4" t="n">
         <v>21</v>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -3953,16 +3976,16 @@
         <v>126.676</v>
       </c>
       <c r="J23" t="n">
-        <v>127.914</v>
+        <v>127.949</v>
       </c>
       <c r="K23" t="n">
-        <v>127.926</v>
+        <v>127.961</v>
       </c>
       <c r="L23" t="n">
-        <v>128.03</v>
+        <v>127.995</v>
       </c>
       <c r="M23" t="n">
-        <v>128.045</v>
+        <v>128.01</v>
       </c>
       <c r="N23" t="n">
         <v>128.968</v>
@@ -3990,7 +4013,7 @@
       </c>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="n">
+      <c r="A24" s="4" t="n">
         <v>22</v>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -4010,16 +4033,16 @@
         <v>126.689</v>
       </c>
       <c r="J24" t="n">
-        <v>127.926</v>
+        <v>127.961</v>
       </c>
       <c r="K24" t="n">
-        <v>127.937</v>
+        <v>127.972</v>
       </c>
       <c r="L24" t="n">
-        <v>128.045</v>
+        <v>128.01</v>
       </c>
       <c r="M24" t="n">
-        <v>128.06</v>
+        <v>128.025</v>
       </c>
       <c r="N24" t="n">
         <v>128.981</v>
@@ -4047,7 +4070,7 @@
       </c>
     </row>
     <row r="25">
-      <c r="A25" s="3" t="n">
+      <c r="A25" s="4" t="n">
         <v>23</v>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -4067,16 +4090,16 @@
         <v>126.703</v>
       </c>
       <c r="J25" t="n">
-        <v>127.937</v>
+        <v>127.972</v>
       </c>
       <c r="K25" t="n">
-        <v>127.948</v>
+        <v>127.983</v>
       </c>
       <c r="L25" t="n">
-        <v>128.06</v>
+        <v>128.025</v>
       </c>
       <c r="M25" t="n">
-        <v>128.075</v>
+        <v>128.04</v>
       </c>
       <c r="N25" t="n">
         <v>128.994</v>
@@ -4104,7 +4127,7 @@
       </c>
     </row>
     <row r="26">
-      <c r="A26" s="3" t="n">
+      <c r="A26" s="4" t="n">
         <v>24</v>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -4124,16 +4147,16 @@
         <v>126.716</v>
       </c>
       <c r="J26" t="n">
-        <v>127.948</v>
+        <v>127.983</v>
       </c>
       <c r="K26" t="n">
-        <v>127.959</v>
+        <v>127.994</v>
       </c>
       <c r="L26" t="n">
-        <v>128.075</v>
+        <v>128.04</v>
       </c>
       <c r="M26" t="n">
-        <v>128.09</v>
+        <v>128.055</v>
       </c>
       <c r="N26" t="n">
         <v>129.007</v>
@@ -4161,7 +4184,7 @@
       </c>
     </row>
     <row r="27">
-      <c r="A27" s="3" t="n">
+      <c r="A27" s="4" t="n">
         <v>25</v>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -4181,16 +4204,16 @@
         <v>126.729</v>
       </c>
       <c r="J27" t="n">
-        <v>127.959</v>
+        <v>127.994</v>
       </c>
       <c r="K27" t="n">
-        <v>127.97</v>
+        <v>128.005</v>
       </c>
       <c r="L27" t="n">
-        <v>128.09</v>
+        <v>128.055</v>
       </c>
       <c r="M27" t="n">
-        <v>128.105</v>
+        <v>128.07</v>
       </c>
       <c r="N27" t="n">
         <v>129.02</v>
@@ -4218,7 +4241,7 @@
       </c>
     </row>
     <row r="28">
-      <c r="A28" s="3" t="n">
+      <c r="A28" s="4" t="n">
         <v>26</v>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -4238,16 +4261,16 @@
         <v>126.742</v>
       </c>
       <c r="J28" t="n">
-        <v>127.97</v>
+        <v>128.005</v>
       </c>
       <c r="K28" t="n">
-        <v>127.982</v>
+        <v>128.017</v>
       </c>
       <c r="L28" t="n">
-        <v>128.105</v>
+        <v>128.07</v>
       </c>
       <c r="M28" t="n">
-        <v>128.12</v>
+        <v>128.085</v>
       </c>
       <c r="N28" t="n">
         <v>129.033</v>
@@ -4275,7 +4298,7 @@
       </c>
     </row>
     <row r="29">
-      <c r="A29" s="3" t="n">
+      <c r="A29" s="4" t="n">
         <v>27</v>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -4295,16 +4318,16 @@
         <v>126.755</v>
       </c>
       <c r="J29" t="n">
-        <v>127.982</v>
+        <v>128.017</v>
       </c>
       <c r="K29" t="n">
-        <v>127.993</v>
+        <v>128.028</v>
       </c>
       <c r="L29" t="n">
-        <v>128.12</v>
+        <v>128.085</v>
       </c>
       <c r="M29" t="n">
-        <v>128.135</v>
+        <v>128.1</v>
       </c>
       <c r="N29" t="n">
         <v>129.046</v>
@@ -4332,7 +4355,7 @@
       </c>
     </row>
     <row r="30">
-      <c r="A30" s="3" t="n">
+      <c r="A30" s="4" t="n">
         <v>28</v>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -4352,16 +4375,16 @@
         <v>126.768</v>
       </c>
       <c r="J30" t="n">
-        <v>127.993</v>
+        <v>128.028</v>
       </c>
       <c r="K30" t="n">
-        <v>128.004</v>
+        <v>128.039</v>
       </c>
       <c r="L30" t="n">
-        <v>128.135</v>
+        <v>128.1</v>
       </c>
       <c r="M30" t="n">
-        <v>128.15</v>
+        <v>128.115</v>
       </c>
       <c r="N30" t="n">
         <v>129.059</v>
@@ -4389,7 +4412,7 @@
       </c>
     </row>
     <row r="31">
-      <c r="A31" s="3" t="n">
+      <c r="A31" s="4" t="n">
         <v>29</v>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -4409,16 +4432,16 @@
         <v>126.782</v>
       </c>
       <c r="J31" t="n">
-        <v>128.004</v>
+        <v>128.039</v>
       </c>
       <c r="K31" t="n">
-        <v>128.015</v>
+        <v>128.05</v>
       </c>
       <c r="L31" t="n">
-        <v>128.15</v>
+        <v>128.115</v>
       </c>
       <c r="M31" t="n">
-        <v>128.165</v>
+        <v>128.13</v>
       </c>
       <c r="N31" t="n">
         <v>129.072</v>
@@ -4446,7 +4469,7 @@
       </c>
     </row>
     <row r="32">
-      <c r="A32" s="3" t="n">
+      <c r="A32" s="4" t="n">
         <v>30</v>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -4466,16 +4489,16 @@
         <v>126.795</v>
       </c>
       <c r="J32" t="n">
-        <v>128.015</v>
+        <v>128.05</v>
       </c>
       <c r="K32" t="n">
-        <v>128.026</v>
+        <v>128.061</v>
       </c>
       <c r="L32" t="n">
-        <v>128.165</v>
+        <v>128.13</v>
       </c>
       <c r="M32" t="n">
-        <v>128.18</v>
+        <v>128.145</v>
       </c>
       <c r="N32" t="n">
         <v>129.085</v>
@@ -4503,7 +4526,7 @@
       </c>
     </row>
     <row r="33">
-      <c r="A33" s="3" t="n">
+      <c r="A33" s="4" t="n">
         <v>31</v>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -4523,16 +4546,16 @@
         <v>126.808</v>
       </c>
       <c r="J33" t="n">
-        <v>128.026</v>
+        <v>128.061</v>
       </c>
       <c r="K33" t="n">
-        <v>128.038</v>
+        <v>128.073</v>
       </c>
       <c r="L33" t="n">
-        <v>128.18</v>
+        <v>128.145</v>
       </c>
       <c r="M33" t="n">
-        <v>128.195</v>
+        <v>128.16</v>
       </c>
       <c r="N33" t="n">
         <v>129.097</v>
@@ -4560,7 +4583,7 @@
       </c>
     </row>
     <row r="34">
-      <c r="A34" s="3" t="n">
+      <c r="A34" s="4" t="n">
         <v>32</v>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -4580,16 +4603,16 @@
         <v>126.821</v>
       </c>
       <c r="J34" t="n">
-        <v>128.038</v>
+        <v>128.073</v>
       </c>
       <c r="K34" t="n">
-        <v>128.049</v>
+        <v>128.084</v>
       </c>
       <c r="L34" t="n">
-        <v>128.195</v>
+        <v>128.16</v>
       </c>
       <c r="M34" t="n">
-        <v>128.21</v>
+        <v>128.175</v>
       </c>
       <c r="N34" t="n">
         <v>129.11</v>
@@ -4617,7 +4640,7 @@
       </c>
     </row>
     <row r="35">
-      <c r="A35" s="3" t="n">
+      <c r="A35" s="4" t="n">
         <v>33</v>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -4637,16 +4660,16 @@
         <v>126.834</v>
       </c>
       <c r="J35" t="n">
-        <v>128.049</v>
+        <v>128.084</v>
       </c>
       <c r="K35" t="n">
-        <v>128.06</v>
+        <v>128.095</v>
       </c>
       <c r="L35" t="n">
-        <v>128.21</v>
+        <v>128.175</v>
       </c>
       <c r="M35" t="n">
-        <v>128.226</v>
+        <v>128.191</v>
       </c>
       <c r="N35" t="n">
         <v>129.123</v>
@@ -4670,7 +4693,7 @@
       </c>
     </row>
     <row r="36">
-      <c r="A36" s="3" t="n">
+      <c r="A36" s="4" t="n">
         <v>34</v>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -4690,16 +4713,16 @@
         <v>126.847</v>
       </c>
       <c r="J36" t="n">
-        <v>128.06</v>
+        <v>128.095</v>
       </c>
       <c r="K36" t="n">
-        <v>128.071</v>
+        <v>128.106</v>
       </c>
       <c r="L36" t="n">
-        <v>128.226</v>
+        <v>128.191</v>
       </c>
       <c r="M36" t="n">
-        <v>128.241</v>
+        <v>128.206</v>
       </c>
       <c r="N36" t="n">
         <v>129.136</v>
@@ -4719,7 +4742,7 @@
       <c r="U36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" s="3" t="n">
+      <c r="A37" s="4" t="n">
         <v>35</v>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -4739,16 +4762,16 @@
         <v>126.86</v>
       </c>
       <c r="J37" t="n">
-        <v>128.071</v>
+        <v>128.106</v>
       </c>
       <c r="K37" t="n">
-        <v>128.083</v>
+        <v>128.118</v>
       </c>
       <c r="L37" t="n">
-        <v>128.241</v>
+        <v>128.206</v>
       </c>
       <c r="M37" t="n">
-        <v>128.256</v>
+        <v>128.221</v>
       </c>
       <c r="N37" t="n">
         <v>129.149</v>
@@ -4768,7 +4791,7 @@
       <c r="U37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" s="3" t="n">
+      <c r="A38" s="4" t="n">
         <v>36</v>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -4788,16 +4811,16 @@
         <v>126.874</v>
       </c>
       <c r="J38" t="n">
-        <v>128.083</v>
+        <v>128.118</v>
       </c>
       <c r="K38" t="n">
-        <v>128.094</v>
+        <v>128.129</v>
       </c>
       <c r="L38" t="n">
-        <v>128.256</v>
+        <v>128.221</v>
       </c>
       <c r="M38" t="n">
-        <v>128.271</v>
+        <v>128.236</v>
       </c>
       <c r="N38" t="n">
         <v>129.162</v>
@@ -4817,7 +4840,7 @@
       <c r="U38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" s="3" t="n">
+      <c r="A39" s="4" t="n">
         <v>37</v>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -4837,16 +4860,16 @@
         <v>126.887</v>
       </c>
       <c r="J39" t="n">
-        <v>128.094</v>
+        <v>128.129</v>
       </c>
       <c r="K39" t="n">
-        <v>128.105</v>
+        <v>128.14</v>
       </c>
       <c r="L39" t="n">
-        <v>128.271</v>
+        <v>128.236</v>
       </c>
       <c r="M39" t="n">
-        <v>128.286</v>
+        <v>128.251</v>
       </c>
       <c r="N39" t="n">
         <v>129.175</v>
@@ -4866,7 +4889,7 @@
       <c r="U39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" s="3" t="n">
+      <c r="A40" s="4" t="n">
         <v>38</v>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -4886,16 +4909,16 @@
         <v>126.9</v>
       </c>
       <c r="J40" t="n">
-        <v>128.105</v>
+        <v>128.14</v>
       </c>
       <c r="K40" t="n">
-        <v>128.116</v>
+        <v>128.151</v>
       </c>
       <c r="L40" t="n">
-        <v>128.286</v>
+        <v>128.251</v>
       </c>
       <c r="M40" t="n">
-        <v>128.301</v>
+        <v>128.266</v>
       </c>
       <c r="N40" t="n">
         <v>129.188</v>
@@ -4915,7 +4938,7 @@
       <c r="U40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" s="3" t="n">
+      <c r="A41" s="4" t="n">
         <v>39</v>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -4935,16 +4958,16 @@
         <v>126.913</v>
       </c>
       <c r="J41" t="n">
-        <v>128.116</v>
+        <v>128.151</v>
       </c>
       <c r="K41" t="n">
-        <v>128.127</v>
+        <v>128.162</v>
       </c>
       <c r="L41" t="n">
-        <v>128.301</v>
+        <v>128.266</v>
       </c>
       <c r="M41" t="n">
-        <v>128.316</v>
+        <v>128.281</v>
       </c>
       <c r="N41" t="n">
         <v>129.201</v>
@@ -4964,7 +4987,7 @@
       <c r="U41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" s="3" t="n">
+      <c r="A42" s="4" t="n">
         <v>40</v>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -4984,16 +5007,16 @@
         <v>126.926</v>
       </c>
       <c r="J42" t="n">
-        <v>128.127</v>
+        <v>128.162</v>
       </c>
       <c r="K42" t="n">
-        <v>128.139</v>
+        <v>128.174</v>
       </c>
       <c r="L42" t="n">
-        <v>128.316</v>
+        <v>128.281</v>
       </c>
       <c r="M42" t="n">
-        <v>128.331</v>
+        <v>128.296</v>
       </c>
       <c r="N42" t="n">
         <v>129.214</v>
@@ -5013,7 +5036,7 @@
       <c r="U42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" s="3" t="n">
+      <c r="A43" s="4" t="n">
         <v>41</v>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -5033,16 +5056,16 @@
         <v>126.939</v>
       </c>
       <c r="J43" t="n">
-        <v>128.139</v>
+        <v>128.174</v>
       </c>
       <c r="K43" t="n">
-        <v>128.15</v>
+        <v>128.185</v>
       </c>
       <c r="L43" t="n">
-        <v>128.331</v>
+        <v>128.296</v>
       </c>
       <c r="M43" t="n">
-        <v>128.346</v>
+        <v>128.311</v>
       </c>
       <c r="N43" t="n">
         <v>129.227</v>
@@ -5062,7 +5085,7 @@
       <c r="U43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" s="3" t="n">
+      <c r="A44" s="4" t="n">
         <v>42</v>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -5082,16 +5105,16 @@
         <v>126.953</v>
       </c>
       <c r="J44" t="n">
-        <v>128.15</v>
+        <v>128.185</v>
       </c>
       <c r="K44" t="n">
-        <v>128.161</v>
+        <v>128.196</v>
       </c>
       <c r="L44" t="n">
-        <v>128.346</v>
+        <v>128.311</v>
       </c>
       <c r="M44" t="n">
-        <v>128.361</v>
+        <v>128.326</v>
       </c>
       <c r="N44" t="n">
         <v>129.24</v>
@@ -5111,7 +5134,7 @@
       <c r="U44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" s="3" t="n">
+      <c r="A45" s="4" t="n">
         <v>43</v>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -5131,16 +5154,16 @@
         <v>126.966</v>
       </c>
       <c r="J45" t="n">
-        <v>128.161</v>
+        <v>128.196</v>
       </c>
       <c r="K45" t="n">
-        <v>128.172</v>
+        <v>128.207</v>
       </c>
       <c r="L45" t="n">
-        <v>128.361</v>
+        <v>128.326</v>
       </c>
       <c r="M45" t="n">
-        <v>128.376</v>
+        <v>128.341</v>
       </c>
       <c r="N45" t="n">
         <v>129.253</v>
@@ -5160,7 +5183,7 @@
       <c r="U45" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" s="3" t="n">
+      <c r="A46" s="4" t="n">
         <v>44</v>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -5180,16 +5203,16 @@
         <v>126.986</v>
       </c>
       <c r="J46" t="n">
-        <v>128.172</v>
+        <v>128.207</v>
       </c>
       <c r="K46" t="n">
-        <v>128.183</v>
+        <v>128.218</v>
       </c>
       <c r="L46" t="n">
-        <v>128.376</v>
+        <v>128.341</v>
       </c>
       <c r="M46" t="n">
-        <v>128.399</v>
+        <v>128.364</v>
       </c>
       <c r="N46" t="n">
         <v>129.266</v>
@@ -5209,7 +5232,7 @@
       <c r="U46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" s="3" t="n">
+      <c r="A47" s="4" t="n">
         <v>45</v>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -5229,10 +5252,10 @@
         <v>127.013</v>
       </c>
       <c r="J47" t="n">
-        <v>128.183</v>
+        <v>128.218</v>
       </c>
       <c r="K47" t="n">
-        <v>128.195</v>
+        <v>128.23</v>
       </c>
       <c r="L47" t="inlineStr"/>
       <c r="M47" t="inlineStr"/>
@@ -5254,7 +5277,7 @@
       <c r="U47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" s="3" t="n">
+      <c r="A48" s="4" t="n">
         <v>46</v>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -5266,10 +5289,10 @@
       <c r="H48" t="inlineStr"/>
       <c r="I48" t="inlineStr"/>
       <c r="J48" t="n">
-        <v>128.195</v>
+        <v>128.23</v>
       </c>
       <c r="K48" t="n">
-        <v>128.206</v>
+        <v>128.241</v>
       </c>
       <c r="L48" t="inlineStr"/>
       <c r="M48" t="inlineStr"/>
@@ -5291,7 +5314,7 @@
       <c r="U48" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" s="3" t="n">
+      <c r="A49" s="4" t="n">
         <v>47</v>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -5303,10 +5326,10 @@
       <c r="H49" t="inlineStr"/>
       <c r="I49" t="inlineStr"/>
       <c r="J49" t="n">
-        <v>128.206</v>
+        <v>128.241</v>
       </c>
       <c r="K49" t="n">
-        <v>128.217</v>
+        <v>128.252</v>
       </c>
       <c r="L49" t="inlineStr"/>
       <c r="M49" t="inlineStr"/>
@@ -5328,7 +5351,7 @@
       <c r="U49" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="A50" s="3" t="n">
+      <c r="A50" s="4" t="n">
         <v>48</v>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -5340,10 +5363,10 @@
       <c r="H50" t="inlineStr"/>
       <c r="I50" t="inlineStr"/>
       <c r="J50" t="n">
-        <v>128.217</v>
+        <v>128.252</v>
       </c>
       <c r="K50" t="n">
-        <v>128.228</v>
+        <v>128.263</v>
       </c>
       <c r="L50" t="inlineStr"/>
       <c r="M50" t="inlineStr"/>
@@ -5365,7 +5388,7 @@
       <c r="U50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" s="3" t="n">
+      <c r="A51" s="4" t="n">
         <v>49</v>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -5377,10 +5400,10 @@
       <c r="H51" t="inlineStr"/>
       <c r="I51" t="inlineStr"/>
       <c r="J51" t="n">
-        <v>128.228</v>
+        <v>128.263</v>
       </c>
       <c r="K51" t="n">
-        <v>128.24</v>
+        <v>128.275</v>
       </c>
       <c r="L51" t="inlineStr"/>
       <c r="M51" t="inlineStr"/>
@@ -5402,7 +5425,7 @@
       <c r="U51" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" s="3" t="n">
+      <c r="A52" s="4" t="n">
         <v>50</v>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -5414,10 +5437,10 @@
       <c r="H52" t="inlineStr"/>
       <c r="I52" t="inlineStr"/>
       <c r="J52" t="n">
-        <v>128.24</v>
+        <v>128.275</v>
       </c>
       <c r="K52" t="n">
-        <v>128.251</v>
+        <v>128.286</v>
       </c>
       <c r="L52" t="inlineStr"/>
       <c r="M52" t="inlineStr"/>
@@ -5439,7 +5462,7 @@
       <c r="U52" t="inlineStr"/>
     </row>
     <row r="53">
-      <c r="A53" s="3" t="n">
+      <c r="A53" s="4" t="n">
         <v>51</v>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -5451,10 +5474,10 @@
       <c r="H53" t="inlineStr"/>
       <c r="I53" t="inlineStr"/>
       <c r="J53" t="n">
-        <v>128.251</v>
+        <v>128.286</v>
       </c>
       <c r="K53" t="n">
-        <v>128.262</v>
+        <v>128.297</v>
       </c>
       <c r="L53" t="inlineStr"/>
       <c r="M53" t="inlineStr"/>
@@ -5476,7 +5499,7 @@
       <c r="U53" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="A54" s="3" t="n">
+      <c r="A54" s="4" t="n">
         <v>52</v>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -5488,10 +5511,10 @@
       <c r="H54" t="inlineStr"/>
       <c r="I54" t="inlineStr"/>
       <c r="J54" t="n">
-        <v>128.262</v>
+        <v>128.297</v>
       </c>
       <c r="K54" t="n">
-        <v>128.273</v>
+        <v>128.308</v>
       </c>
       <c r="L54" t="inlineStr"/>
       <c r="M54" t="inlineStr"/>
@@ -5509,7 +5532,7 @@
       <c r="U54" t="inlineStr"/>
     </row>
     <row r="55">
-      <c r="A55" s="3" t="n">
+      <c r="A55" s="4" t="n">
         <v>53</v>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -5521,10 +5544,10 @@
       <c r="H55" t="inlineStr"/>
       <c r="I55" t="inlineStr"/>
       <c r="J55" t="n">
-        <v>128.273</v>
+        <v>128.308</v>
       </c>
       <c r="K55" t="n">
-        <v>128.284</v>
+        <v>128.319</v>
       </c>
       <c r="L55" t="inlineStr"/>
       <c r="M55" t="inlineStr"/>
@@ -5542,7 +5565,7 @@
       <c r="U55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" s="3" t="n">
+      <c r="A56" s="4" t="n">
         <v>54</v>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -5554,10 +5577,10 @@
       <c r="H56" t="inlineStr"/>
       <c r="I56" t="inlineStr"/>
       <c r="J56" t="n">
-        <v>128.284</v>
+        <v>128.319</v>
       </c>
       <c r="K56" t="n">
-        <v>128.296</v>
+        <v>128.331</v>
       </c>
       <c r="L56" t="inlineStr"/>
       <c r="M56" t="inlineStr"/>
@@ -5575,7 +5598,7 @@
       <c r="U56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" s="3" t="n">
+      <c r="A57" s="4" t="n">
         <v>55</v>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -5587,10 +5610,10 @@
       <c r="H57" t="inlineStr"/>
       <c r="I57" t="inlineStr"/>
       <c r="J57" t="n">
-        <v>128.296</v>
+        <v>128.331</v>
       </c>
       <c r="K57" t="n">
-        <v>128.307</v>
+        <v>128.342</v>
       </c>
       <c r="L57" t="inlineStr"/>
       <c r="M57" t="inlineStr"/>
@@ -5608,7 +5631,7 @@
       <c r="U57" t="inlineStr"/>
     </row>
     <row r="58">
-      <c r="A58" s="3" t="n">
+      <c r="A58" s="4" t="n">
         <v>56</v>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -5620,10 +5643,10 @@
       <c r="H58" t="inlineStr"/>
       <c r="I58" t="inlineStr"/>
       <c r="J58" t="n">
-        <v>128.307</v>
+        <v>128.342</v>
       </c>
       <c r="K58" t="n">
-        <v>128.325</v>
+        <v>128.36</v>
       </c>
       <c r="L58" t="inlineStr"/>
       <c r="M58" t="inlineStr"/>
@@ -5641,7 +5664,7 @@
       <c r="U58" t="inlineStr"/>
     </row>
     <row r="59">
-      <c r="A59" s="3" t="n">
+      <c r="A59" s="4" t="n">
         <v>57</v>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -5670,7 +5693,7 @@
       <c r="U59" t="inlineStr"/>
     </row>
     <row r="60">
-      <c r="A60" s="3" t="n">
+      <c r="A60" s="4" t="n">
         <v>58</v>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -5699,7 +5722,7 @@
       <c r="U60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" s="3" t="n">
+      <c r="A61" s="4" t="n">
         <v>59</v>
       </c>
       <c r="B61" t="inlineStr"/>

</xml_diff>

<commit_message>
catchup on misc minor changes
</commit_message>
<xml_diff>
--- a/data/sampling/water_iso/water_iso_depths.xlsx
+++ b/data/sampling/water_iso/water_iso_depths.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="1060" yWindow="760" windowWidth="23580" windowHeight="18880" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="18140" yWindow="-22240" windowWidth="23580" windowHeight="18880" tabRatio="600" firstSheet="0" activeTab="1" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="sample_thicknesses" sheetId="1" state="visible" r:id="rId1"/>
@@ -18,7 +18,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="4">
+  <fonts count="3">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -32,11 +32,6 @@
       <color rgb="FF000000"/>
       <sz val="12"/>
       <scheme val="minor"/>
-    </font>
-    <font>
-      <name val="Aptos Narrow"/>
-      <b val="1"/>
-      <sz val="12"/>
     </font>
     <font>
       <b val="1"/>
@@ -56,27 +51,12 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom style="thin">
-        <color auto="1"/>
-      </bottom>
       <diagonal/>
     </border>
     <border>
@@ -89,14 +69,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -496,12 +473,12 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K61"/>
+  <dimension ref="A1:L61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A6" sqref="A6"/>
-      <selection pane="topRight" activeCell="E2" sqref="E2"/>
+      <selection pane="topRight" activeCell="L18" sqref="L18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="19.33203125" defaultRowHeight="16"/>
@@ -522,12 +499,12 @@
           <t>alhic1901-230_4-r</t>
         </is>
       </c>
-      <c r="D1" s="2" t="inlineStr">
+      <c r="D1" t="inlineStr">
         <is>
           <t>alhic2302-155_2-r</t>
         </is>
       </c>
-      <c r="E1" s="2" t="inlineStr">
+      <c r="E1" t="inlineStr">
         <is>
           <t>alhic2302-155_2-l</t>
         </is>
@@ -560,6 +537,11 @@
       <c r="K1" t="inlineStr">
         <is>
           <t>alhic2302-159_3-r</t>
+        </is>
+      </c>
+      <c r="L1" t="inlineStr">
+        <is>
+          <t>alhic2302-155_2-stick2</t>
         </is>
       </c>
     </row>
@@ -597,6 +579,9 @@
       <c r="K2" t="n">
         <v>11</v>
       </c>
+      <c r="L2" t="n">
+        <v>38.9322</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -632,6 +617,9 @@
       <c r="K3" t="n">
         <v>11</v>
       </c>
+      <c r="L3" t="n">
+        <v>39.5556</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -667,6 +655,9 @@
       <c r="K4" t="n">
         <v>11</v>
       </c>
+      <c r="L4" t="n">
+        <v>39.8722</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -702,6 +693,9 @@
       <c r="K5" t="n">
         <v>11</v>
       </c>
+      <c r="L5" t="n">
+        <v>37.795</v>
+      </c>
     </row>
     <row r="6">
       <c r="A6" t="n">
@@ -737,6 +731,9 @@
       <c r="K6" t="n">
         <v>11</v>
       </c>
+      <c r="L6" t="n">
+        <v>36.755</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -772,6 +769,9 @@
       <c r="K7" t="n">
         <v>11</v>
       </c>
+      <c r="L7" t="n">
+        <v>37.586</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -807,6 +807,9 @@
       <c r="K8" t="n">
         <v>11</v>
       </c>
+      <c r="L8" t="n">
+        <v>37.583</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -842,6 +845,9 @@
       <c r="K9" t="n">
         <v>11</v>
       </c>
+      <c r="L9" t="n">
+        <v>38.054</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -877,6 +883,9 @@
       <c r="K10" t="n">
         <v>11</v>
       </c>
+      <c r="L10" t="n">
+        <v>37.225</v>
+      </c>
     </row>
     <row r="11">
       <c r="A11" t="n">
@@ -912,6 +921,9 @@
       <c r="K11" t="n">
         <v>11</v>
       </c>
+      <c r="L11" t="n">
+        <v>35.913</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" t="n">
@@ -947,6 +959,9 @@
       <c r="K12" t="n">
         <v>11</v>
       </c>
+      <c r="L12" t="n">
+        <v>36.649</v>
+      </c>
     </row>
     <row r="13">
       <c r="A13" t="n">
@@ -981,6 +996,9 @@
       </c>
       <c r="K13" t="n">
         <v>11</v>
+      </c>
+      <c r="L13" t="n">
+        <v>35.966</v>
       </c>
     </row>
     <row r="14">
@@ -1017,6 +1035,9 @@
       <c r="K14" t="n">
         <v>11</v>
       </c>
+      <c r="L14" t="n">
+        <v>35.644</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -1052,6 +1073,9 @@
       <c r="K15" t="n">
         <v>11</v>
       </c>
+      <c r="L15" t="n">
+        <v>33.734</v>
+      </c>
     </row>
     <row r="16">
       <c r="A16" t="n">
@@ -1087,6 +1111,9 @@
       <c r="K16" t="n">
         <v>11</v>
       </c>
+      <c r="L16" t="n">
+        <v>35.243</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -1121,6 +1148,9 @@
       </c>
       <c r="K17" t="n">
         <v>11</v>
+      </c>
+      <c r="L17" t="n">
+        <v>31.893</v>
       </c>
     </row>
     <row r="18">
@@ -2104,10 +2134,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:I11"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2488,6 +2518,40 @@
       <c r="I11" t="inlineStr">
         <is>
           <t>done</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>alhic2302-155_2-stick2</t>
+        </is>
+      </c>
+      <c r="B12" t="n">
+        <v>588.4</v>
+      </c>
+      <c r="C12" t="n">
+        <v>126.4</v>
+      </c>
+      <c r="D12">
+        <f>0+2+16</f>
+        <v/>
+      </c>
+      <c r="E12" t="n">
+        <v>32</v>
+      </c>
+      <c r="F12" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" t="n">
+        <v>61</v>
+      </c>
+      <c r="H12" t="n">
+        <v>31</v>
+      </c>
+      <c r="I12" t="inlineStr">
+        <is>
+          <t>MUST ADD 16mm to offset to acount for lost section at top of stick</t>
         </is>
       </c>
     </row>
@@ -2502,7 +2566,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:U61"/>
+  <dimension ref="A1:W61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -2511,109 +2575,119 @@
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
     <row r="1">
-      <c r="B1" s="4" t="inlineStr">
+      <c r="B1" s="3" t="inlineStr">
         <is>
           <t>alhic1901-230_4-l_td</t>
         </is>
       </c>
-      <c r="C1" s="4" t="inlineStr">
+      <c r="C1" s="3" t="inlineStr">
         <is>
           <t>alhic1901-230_4-l_bd</t>
         </is>
       </c>
-      <c r="D1" s="4" t="inlineStr">
+      <c r="D1" s="3" t="inlineStr">
         <is>
           <t>alhic1901-230_4-r_td</t>
         </is>
       </c>
-      <c r="E1" s="4" t="inlineStr">
+      <c r="E1" s="3" t="inlineStr">
         <is>
           <t>alhic1901-230_4-r_bd</t>
         </is>
       </c>
-      <c r="F1" s="4" t="inlineStr">
+      <c r="F1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-155_2-r_td</t>
         </is>
       </c>
-      <c r="G1" s="4" t="inlineStr">
+      <c r="G1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-155_2-r_bd</t>
         </is>
       </c>
-      <c r="H1" s="4" t="inlineStr">
+      <c r="H1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-155_2-l_td</t>
         </is>
       </c>
-      <c r="I1" s="4" t="inlineStr">
+      <c r="I1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-155_2-l_bd</t>
         </is>
       </c>
-      <c r="J1" s="4" t="inlineStr">
+      <c r="J1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-156_2-l_td</t>
         </is>
       </c>
-      <c r="K1" s="4" t="inlineStr">
+      <c r="K1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-156_2-l_bd</t>
         </is>
       </c>
-      <c r="L1" s="4" t="inlineStr">
+      <c r="L1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-156_2-r_td</t>
         </is>
       </c>
-      <c r="M1" s="4" t="inlineStr">
+      <c r="M1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-156_2-r_bd</t>
         </is>
       </c>
-      <c r="N1" s="4" t="inlineStr">
+      <c r="N1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-158-l_td</t>
         </is>
       </c>
-      <c r="O1" s="4" t="inlineStr">
+      <c r="O1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-158-l_bd</t>
         </is>
       </c>
-      <c r="P1" s="4" t="inlineStr">
+      <c r="P1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-158-r_td</t>
         </is>
       </c>
-      <c r="Q1" s="4" t="inlineStr">
+      <c r="Q1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-158-r_bd</t>
         </is>
       </c>
-      <c r="R1" s="4" t="inlineStr">
+      <c r="R1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-159_3-l_td</t>
         </is>
       </c>
-      <c r="S1" s="4" t="inlineStr">
+      <c r="S1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-159_3-l_bd</t>
         </is>
       </c>
-      <c r="T1" s="4" t="inlineStr">
+      <c r="T1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-159_3-r_td</t>
         </is>
       </c>
-      <c r="U1" s="4" t="inlineStr">
+      <c r="U1" s="3" t="inlineStr">
         <is>
           <t>alhic2302-159_3-r_bd</t>
         </is>
       </c>
+      <c r="V1" s="3" t="inlineStr">
+        <is>
+          <t>alhic2302-155_2-stick2_td</t>
+        </is>
+      </c>
+      <c r="W1" s="3" t="inlineStr">
+        <is>
+          <t>alhic2302-155_2-stick2_bd</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" s="4" t="n">
+      <c r="A2" s="3" t="n">
         <v>0</v>
       </c>
       <c r="B2" t="n">
@@ -2676,9 +2750,15 @@
       <c r="U2" t="n">
         <v>129.834</v>
       </c>
+      <c r="V2" t="n">
+        <v>126.418</v>
+      </c>
+      <c r="W2" t="n">
+        <v>126.457</v>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" s="4" t="n">
+      <c r="A3" s="3" t="n">
         <v>1</v>
       </c>
       <c r="B3" t="n">
@@ -2741,9 +2821,15 @@
       <c r="U3" t="n">
         <v>129.846</v>
       </c>
+      <c r="V3" t="n">
+        <v>126.457</v>
+      </c>
+      <c r="W3" t="n">
+        <v>126.496</v>
+      </c>
     </row>
     <row r="4">
-      <c r="A4" s="4" t="n">
+      <c r="A4" s="3" t="n">
         <v>2</v>
       </c>
       <c r="B4" t="n">
@@ -2806,9 +2892,15 @@
       <c r="U4" t="n">
         <v>129.857</v>
       </c>
+      <c r="V4" t="n">
+        <v>126.496</v>
+      </c>
+      <c r="W4" t="n">
+        <v>126.536</v>
+      </c>
     </row>
     <row r="5">
-      <c r="A5" s="4" t="n">
+      <c r="A5" s="3" t="n">
         <v>3</v>
       </c>
       <c r="B5" t="n">
@@ -2871,9 +2963,15 @@
       <c r="U5" t="n">
         <v>129.869</v>
       </c>
+      <c r="V5" t="n">
+        <v>126.536</v>
+      </c>
+      <c r="W5" t="n">
+        <v>126.574</v>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" s="4" t="n">
+      <c r="A6" s="3" t="n">
         <v>4</v>
       </c>
       <c r="B6" t="n">
@@ -2936,9 +3034,15 @@
       <c r="U6" t="n">
         <v>129.88</v>
       </c>
+      <c r="V6" t="n">
+        <v>126.574</v>
+      </c>
+      <c r="W6" t="n">
+        <v>126.611</v>
+      </c>
     </row>
     <row r="7">
-      <c r="A7" s="4" t="n">
+      <c r="A7" s="3" t="n">
         <v>5</v>
       </c>
       <c r="B7" t="n">
@@ -3001,9 +3105,15 @@
       <c r="U7" t="n">
         <v>129.892</v>
       </c>
+      <c r="V7" t="n">
+        <v>126.611</v>
+      </c>
+      <c r="W7" t="n">
+        <v>126.648</v>
+      </c>
     </row>
     <row r="8">
-      <c r="A8" s="4" t="n">
+      <c r="A8" s="3" t="n">
         <v>6</v>
       </c>
       <c r="B8" t="n">
@@ -3066,9 +3176,15 @@
       <c r="U8" t="n">
         <v>129.903</v>
       </c>
+      <c r="V8" t="n">
+        <v>126.648</v>
+      </c>
+      <c r="W8" t="n">
+        <v>126.686</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="4" t="n">
+      <c r="A9" s="3" t="n">
         <v>7</v>
       </c>
       <c r="B9" t="n">
@@ -3131,9 +3247,15 @@
       <c r="U9" t="n">
         <v>129.915</v>
       </c>
+      <c r="V9" t="n">
+        <v>126.686</v>
+      </c>
+      <c r="W9" t="n">
+        <v>126.724</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="4" t="n">
+      <c r="A10" s="3" t="n">
         <v>8</v>
       </c>
       <c r="B10" t="n">
@@ -3196,9 +3318,15 @@
       <c r="U10" t="n">
         <v>129.926</v>
       </c>
+      <c r="V10" t="n">
+        <v>126.724</v>
+      </c>
+      <c r="W10" t="n">
+        <v>126.761</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="4" t="n">
+      <c r="A11" s="3" t="n">
         <v>9</v>
       </c>
       <c r="B11" t="n">
@@ -3261,9 +3389,15 @@
       <c r="U11" t="n">
         <v>129.938</v>
       </c>
+      <c r="V11" t="n">
+        <v>126.761</v>
+      </c>
+      <c r="W11" t="n">
+        <v>126.797</v>
+      </c>
     </row>
     <row r="12">
-      <c r="A12" s="4" t="n">
+      <c r="A12" s="3" t="n">
         <v>10</v>
       </c>
       <c r="B12" t="n">
@@ -3326,9 +3460,15 @@
       <c r="U12" t="n">
         <v>129.949</v>
       </c>
+      <c r="V12" t="n">
+        <v>126.797</v>
+      </c>
+      <c r="W12" t="n">
+        <v>126.834</v>
+      </c>
     </row>
     <row r="13">
-      <c r="A13" s="4" t="n">
+      <c r="A13" s="3" t="n">
         <v>11</v>
       </c>
       <c r="B13" t="n">
@@ -3391,9 +3531,15 @@
       <c r="U13" t="n">
         <v>129.961</v>
       </c>
+      <c r="V13" t="n">
+        <v>126.834</v>
+      </c>
+      <c r="W13" t="n">
+        <v>126.87</v>
+      </c>
     </row>
     <row r="14">
-      <c r="A14" s="4" t="n">
+      <c r="A14" s="3" t="n">
         <v>12</v>
       </c>
       <c r="B14" t="n">
@@ -3456,9 +3602,15 @@
       <c r="U14" t="n">
         <v>129.972</v>
       </c>
+      <c r="V14" t="n">
+        <v>126.87</v>
+      </c>
+      <c r="W14" t="n">
+        <v>126.906</v>
+      </c>
     </row>
     <row r="15">
-      <c r="A15" s="4" t="n">
+      <c r="A15" s="3" t="n">
         <v>13</v>
       </c>
       <c r="B15" t="n">
@@ -3521,9 +3673,15 @@
       <c r="U15" t="n">
         <v>129.984</v>
       </c>
+      <c r="V15" t="n">
+        <v>126.906</v>
+      </c>
+      <c r="W15" t="n">
+        <v>126.939</v>
+      </c>
     </row>
     <row r="16">
-      <c r="A16" s="4" t="n">
+      <c r="A16" s="3" t="n">
         <v>14</v>
       </c>
       <c r="B16" t="n">
@@ -3586,9 +3744,15 @@
       <c r="U16" t="n">
         <v>129.995</v>
       </c>
+      <c r="V16" t="n">
+        <v>126.939</v>
+      </c>
+      <c r="W16" t="n">
+        <v>126.975</v>
+      </c>
     </row>
     <row r="17">
-      <c r="A17" s="4" t="n">
+      <c r="A17" s="3" t="n">
         <v>15</v>
       </c>
       <c r="B17" t="n">
@@ -3651,9 +3815,15 @@
       <c r="U17" t="n">
         <v>130.007</v>
       </c>
+      <c r="V17" t="n">
+        <v>126.975</v>
+      </c>
+      <c r="W17" t="n">
+        <v>127.006</v>
+      </c>
     </row>
     <row r="18">
-      <c r="A18" s="4" t="n">
+      <c r="A18" s="3" t="n">
         <v>16</v>
       </c>
       <c r="B18" t="n">
@@ -3716,9 +3886,11 @@
       <c r="U18" t="n">
         <v>130.018</v>
       </c>
+      <c r="V18" t="inlineStr"/>
+      <c r="W18" t="inlineStr"/>
     </row>
     <row r="19">
-      <c r="A19" s="4" t="n">
+      <c r="A19" s="3" t="n">
         <v>17</v>
       </c>
       <c r="B19" t="n">
@@ -3781,9 +3953,11 @@
       <c r="U19" t="n">
         <v>130.03</v>
       </c>
+      <c r="V19" t="inlineStr"/>
+      <c r="W19" t="inlineStr"/>
     </row>
     <row r="20">
-      <c r="A20" s="4" t="n">
+      <c r="A20" s="3" t="n">
         <v>18</v>
       </c>
       <c r="B20" t="inlineStr"/>
@@ -3842,9 +4016,11 @@
       <c r="U20" t="n">
         <v>130.041</v>
       </c>
+      <c r="V20" t="inlineStr"/>
+      <c r="W20" t="inlineStr"/>
     </row>
     <row r="21">
-      <c r="A21" s="4" t="n">
+      <c r="A21" s="3" t="n">
         <v>19</v>
       </c>
       <c r="B21" t="inlineStr"/>
@@ -3899,9 +4075,11 @@
       <c r="U21" t="n">
         <v>130.053</v>
       </c>
+      <c r="V21" t="inlineStr"/>
+      <c r="W21" t="inlineStr"/>
     </row>
     <row r="22">
-      <c r="A22" s="4" t="n">
+      <c r="A22" s="3" t="n">
         <v>20</v>
       </c>
       <c r="B22" t="inlineStr"/>
@@ -3956,9 +4134,11 @@
       <c r="U22" t="n">
         <v>130.064</v>
       </c>
+      <c r="V22" t="inlineStr"/>
+      <c r="W22" t="inlineStr"/>
     </row>
     <row r="23">
-      <c r="A23" s="4" t="n">
+      <c r="A23" s="3" t="n">
         <v>21</v>
       </c>
       <c r="B23" t="inlineStr"/>
@@ -4013,9 +4193,11 @@
       <c r="U23" t="n">
         <v>130.076</v>
       </c>
+      <c r="V23" t="inlineStr"/>
+      <c r="W23" t="inlineStr"/>
     </row>
     <row r="24">
-      <c r="A24" s="4" t="n">
+      <c r="A24" s="3" t="n">
         <v>22</v>
       </c>
       <c r="B24" t="inlineStr"/>
@@ -4070,9 +4252,11 @@
       <c r="U24" t="n">
         <v>130.087</v>
       </c>
+      <c r="V24" t="inlineStr"/>
+      <c r="W24" t="inlineStr"/>
     </row>
     <row r="25">
-      <c r="A25" s="4" t="n">
+      <c r="A25" s="3" t="n">
         <v>23</v>
       </c>
       <c r="B25" t="inlineStr"/>
@@ -4127,9 +4311,11 @@
       <c r="U25" t="n">
         <v>130.099</v>
       </c>
+      <c r="V25" t="inlineStr"/>
+      <c r="W25" t="inlineStr"/>
     </row>
     <row r="26">
-      <c r="A26" s="4" t="n">
+      <c r="A26" s="3" t="n">
         <v>24</v>
       </c>
       <c r="B26" t="inlineStr"/>
@@ -4184,9 +4370,11 @@
       <c r="U26" t="n">
         <v>130.11</v>
       </c>
+      <c r="V26" t="inlineStr"/>
+      <c r="W26" t="inlineStr"/>
     </row>
     <row r="27">
-      <c r="A27" s="4" t="n">
+      <c r="A27" s="3" t="n">
         <v>25</v>
       </c>
       <c r="B27" t="inlineStr"/>
@@ -4241,9 +4429,11 @@
       <c r="U27" t="n">
         <v>130.122</v>
       </c>
+      <c r="V27" t="inlineStr"/>
+      <c r="W27" t="inlineStr"/>
     </row>
     <row r="28">
-      <c r="A28" s="4" t="n">
+      <c r="A28" s="3" t="n">
         <v>26</v>
       </c>
       <c r="B28" t="inlineStr"/>
@@ -4298,9 +4488,11 @@
       <c r="U28" t="n">
         <v>130.133</v>
       </c>
+      <c r="V28" t="inlineStr"/>
+      <c r="W28" t="inlineStr"/>
     </row>
     <row r="29">
-      <c r="A29" s="4" t="n">
+      <c r="A29" s="3" t="n">
         <v>27</v>
       </c>
       <c r="B29" t="inlineStr"/>
@@ -4355,9 +4547,11 @@
       <c r="U29" t="n">
         <v>130.145</v>
       </c>
+      <c r="V29" t="inlineStr"/>
+      <c r="W29" t="inlineStr"/>
     </row>
     <row r="30">
-      <c r="A30" s="4" t="n">
+      <c r="A30" s="3" t="n">
         <v>28</v>
       </c>
       <c r="B30" t="inlineStr"/>
@@ -4412,9 +4606,11 @@
       <c r="U30" t="n">
         <v>130.156</v>
       </c>
+      <c r="V30" t="inlineStr"/>
+      <c r="W30" t="inlineStr"/>
     </row>
     <row r="31">
-      <c r="A31" s="4" t="n">
+      <c r="A31" s="3" t="n">
         <v>29</v>
       </c>
       <c r="B31" t="inlineStr"/>
@@ -4469,9 +4665,11 @@
       <c r="U31" t="n">
         <v>130.168</v>
       </c>
+      <c r="V31" t="inlineStr"/>
+      <c r="W31" t="inlineStr"/>
     </row>
     <row r="32">
-      <c r="A32" s="4" t="n">
+      <c r="A32" s="3" t="n">
         <v>30</v>
       </c>
       <c r="B32" t="inlineStr"/>
@@ -4526,9 +4724,11 @@
       <c r="U32" t="n">
         <v>130.179</v>
       </c>
+      <c r="V32" t="inlineStr"/>
+      <c r="W32" t="inlineStr"/>
     </row>
     <row r="33">
-      <c r="A33" s="4" t="n">
+      <c r="A33" s="3" t="n">
         <v>31</v>
       </c>
       <c r="B33" t="inlineStr"/>
@@ -4583,9 +4783,11 @@
       <c r="U33" t="n">
         <v>130.191</v>
       </c>
+      <c r="V33" t="inlineStr"/>
+      <c r="W33" t="inlineStr"/>
     </row>
     <row r="34">
-      <c r="A34" s="4" t="n">
+      <c r="A34" s="3" t="n">
         <v>32</v>
       </c>
       <c r="B34" t="inlineStr"/>
@@ -4640,9 +4842,11 @@
       <c r="U34" t="n">
         <v>130.202</v>
       </c>
+      <c r="V34" t="inlineStr"/>
+      <c r="W34" t="inlineStr"/>
     </row>
     <row r="35">
-      <c r="A35" s="4" t="n">
+      <c r="A35" s="3" t="n">
         <v>33</v>
       </c>
       <c r="B35" t="inlineStr"/>
@@ -4693,9 +4897,11 @@
       <c r="U35" t="n">
         <v>130.218</v>
       </c>
+      <c r="V35" t="inlineStr"/>
+      <c r="W35" t="inlineStr"/>
     </row>
     <row r="36">
-      <c r="A36" s="4" t="n">
+      <c r="A36" s="3" t="n">
         <v>34</v>
       </c>
       <c r="B36" t="inlineStr"/>
@@ -4742,9 +4948,11 @@
       <c r="S36" t="inlineStr"/>
       <c r="T36" t="inlineStr"/>
       <c r="U36" t="inlineStr"/>
+      <c r="V36" t="inlineStr"/>
+      <c r="W36" t="inlineStr"/>
     </row>
     <row r="37">
-      <c r="A37" s="4" t="n">
+      <c r="A37" s="3" t="n">
         <v>35</v>
       </c>
       <c r="B37" t="inlineStr"/>
@@ -4791,9 +4999,11 @@
       <c r="S37" t="inlineStr"/>
       <c r="T37" t="inlineStr"/>
       <c r="U37" t="inlineStr"/>
+      <c r="V37" t="inlineStr"/>
+      <c r="W37" t="inlineStr"/>
     </row>
     <row r="38">
-      <c r="A38" s="4" t="n">
+      <c r="A38" s="3" t="n">
         <v>36</v>
       </c>
       <c r="B38" t="inlineStr"/>
@@ -4840,9 +5050,11 @@
       <c r="S38" t="inlineStr"/>
       <c r="T38" t="inlineStr"/>
       <c r="U38" t="inlineStr"/>
+      <c r="V38" t="inlineStr"/>
+      <c r="W38" t="inlineStr"/>
     </row>
     <row r="39">
-      <c r="A39" s="4" t="n">
+      <c r="A39" s="3" t="n">
         <v>37</v>
       </c>
       <c r="B39" t="inlineStr"/>
@@ -4889,9 +5101,11 @@
       <c r="S39" t="inlineStr"/>
       <c r="T39" t="inlineStr"/>
       <c r="U39" t="inlineStr"/>
+      <c r="V39" t="inlineStr"/>
+      <c r="W39" t="inlineStr"/>
     </row>
     <row r="40">
-      <c r="A40" s="4" t="n">
+      <c r="A40" s="3" t="n">
         <v>38</v>
       </c>
       <c r="B40" t="inlineStr"/>
@@ -4938,9 +5152,11 @@
       <c r="S40" t="inlineStr"/>
       <c r="T40" t="inlineStr"/>
       <c r="U40" t="inlineStr"/>
+      <c r="V40" t="inlineStr"/>
+      <c r="W40" t="inlineStr"/>
     </row>
     <row r="41">
-      <c r="A41" s="4" t="n">
+      <c r="A41" s="3" t="n">
         <v>39</v>
       </c>
       <c r="B41" t="inlineStr"/>
@@ -4987,9 +5203,11 @@
       <c r="S41" t="inlineStr"/>
       <c r="T41" t="inlineStr"/>
       <c r="U41" t="inlineStr"/>
+      <c r="V41" t="inlineStr"/>
+      <c r="W41" t="inlineStr"/>
     </row>
     <row r="42">
-      <c r="A42" s="4" t="n">
+      <c r="A42" s="3" t="n">
         <v>40</v>
       </c>
       <c r="B42" t="inlineStr"/>
@@ -5036,9 +5254,11 @@
       <c r="S42" t="inlineStr"/>
       <c r="T42" t="inlineStr"/>
       <c r="U42" t="inlineStr"/>
+      <c r="V42" t="inlineStr"/>
+      <c r="W42" t="inlineStr"/>
     </row>
     <row r="43">
-      <c r="A43" s="4" t="n">
+      <c r="A43" s="3" t="n">
         <v>41</v>
       </c>
       <c r="B43" t="inlineStr"/>
@@ -5085,9 +5305,11 @@
       <c r="S43" t="inlineStr"/>
       <c r="T43" t="inlineStr"/>
       <c r="U43" t="inlineStr"/>
+      <c r="V43" t="inlineStr"/>
+      <c r="W43" t="inlineStr"/>
     </row>
     <row r="44">
-      <c r="A44" s="4" t="n">
+      <c r="A44" s="3" t="n">
         <v>42</v>
       </c>
       <c r="B44" t="inlineStr"/>
@@ -5134,9 +5356,11 @@
       <c r="S44" t="inlineStr"/>
       <c r="T44" t="inlineStr"/>
       <c r="U44" t="inlineStr"/>
+      <c r="V44" t="inlineStr"/>
+      <c r="W44" t="inlineStr"/>
     </row>
     <row r="45">
-      <c r="A45" s="4" t="n">
+      <c r="A45" s="3" t="n">
         <v>43</v>
       </c>
       <c r="B45" t="inlineStr"/>
@@ -5183,9 +5407,11 @@
       <c r="S45" t="inlineStr"/>
       <c r="T45" t="inlineStr"/>
       <c r="U45" t="inlineStr"/>
+      <c r="V45" t="inlineStr"/>
+      <c r="W45" t="inlineStr"/>
     </row>
     <row r="46">
-      <c r="A46" s="4" t="n">
+      <c r="A46" s="3" t="n">
         <v>44</v>
       </c>
       <c r="B46" t="inlineStr"/>
@@ -5232,9 +5458,11 @@
       <c r="S46" t="inlineStr"/>
       <c r="T46" t="inlineStr"/>
       <c r="U46" t="inlineStr"/>
+      <c r="V46" t="inlineStr"/>
+      <c r="W46" t="inlineStr"/>
     </row>
     <row r="47">
-      <c r="A47" s="4" t="n">
+      <c r="A47" s="3" t="n">
         <v>45</v>
       </c>
       <c r="B47" t="inlineStr"/>
@@ -5277,9 +5505,11 @@
       <c r="S47" t="inlineStr"/>
       <c r="T47" t="inlineStr"/>
       <c r="U47" t="inlineStr"/>
+      <c r="V47" t="inlineStr"/>
+      <c r="W47" t="inlineStr"/>
     </row>
     <row r="48">
-      <c r="A48" s="4" t="n">
+      <c r="A48" s="3" t="n">
         <v>46</v>
       </c>
       <c r="B48" t="inlineStr"/>
@@ -5314,9 +5544,11 @@
       <c r="S48" t="inlineStr"/>
       <c r="T48" t="inlineStr"/>
       <c r="U48" t="inlineStr"/>
+      <c r="V48" t="inlineStr"/>
+      <c r="W48" t="inlineStr"/>
     </row>
     <row r="49">
-      <c r="A49" s="4" t="n">
+      <c r="A49" s="3" t="n">
         <v>47</v>
       </c>
       <c r="B49" t="inlineStr"/>
@@ -5351,9 +5583,11 @@
       <c r="S49" t="inlineStr"/>
       <c r="T49" t="inlineStr"/>
       <c r="U49" t="inlineStr"/>
+      <c r="V49" t="inlineStr"/>
+      <c r="W49" t="inlineStr"/>
     </row>
     <row r="50">
-      <c r="A50" s="4" t="n">
+      <c r="A50" s="3" t="n">
         <v>48</v>
       </c>
       <c r="B50" t="inlineStr"/>
@@ -5388,9 +5622,11 @@
       <c r="S50" t="inlineStr"/>
       <c r="T50" t="inlineStr"/>
       <c r="U50" t="inlineStr"/>
+      <c r="V50" t="inlineStr"/>
+      <c r="W50" t="inlineStr"/>
     </row>
     <row r="51">
-      <c r="A51" s="4" t="n">
+      <c r="A51" s="3" t="n">
         <v>49</v>
       </c>
       <c r="B51" t="inlineStr"/>
@@ -5425,9 +5661,11 @@
       <c r="S51" t="inlineStr"/>
       <c r="T51" t="inlineStr"/>
       <c r="U51" t="inlineStr"/>
+      <c r="V51" t="inlineStr"/>
+      <c r="W51" t="inlineStr"/>
     </row>
     <row r="52">
-      <c r="A52" s="4" t="n">
+      <c r="A52" s="3" t="n">
         <v>50</v>
       </c>
       <c r="B52" t="inlineStr"/>
@@ -5462,9 +5700,11 @@
       <c r="S52" t="inlineStr"/>
       <c r="T52" t="inlineStr"/>
       <c r="U52" t="inlineStr"/>
+      <c r="V52" t="inlineStr"/>
+      <c r="W52" t="inlineStr"/>
     </row>
     <row r="53">
-      <c r="A53" s="4" t="n">
+      <c r="A53" s="3" t="n">
         <v>51</v>
       </c>
       <c r="B53" t="inlineStr"/>
@@ -5499,9 +5739,11 @@
       <c r="S53" t="inlineStr"/>
       <c r="T53" t="inlineStr"/>
       <c r="U53" t="inlineStr"/>
+      <c r="V53" t="inlineStr"/>
+      <c r="W53" t="inlineStr"/>
     </row>
     <row r="54">
-      <c r="A54" s="4" t="n">
+      <c r="A54" s="3" t="n">
         <v>52</v>
       </c>
       <c r="B54" t="inlineStr"/>
@@ -5532,9 +5774,11 @@
       <c r="S54" t="inlineStr"/>
       <c r="T54" t="inlineStr"/>
       <c r="U54" t="inlineStr"/>
+      <c r="V54" t="inlineStr"/>
+      <c r="W54" t="inlineStr"/>
     </row>
     <row r="55">
-      <c r="A55" s="4" t="n">
+      <c r="A55" s="3" t="n">
         <v>53</v>
       </c>
       <c r="B55" t="inlineStr"/>
@@ -5565,9 +5809,11 @@
       <c r="S55" t="inlineStr"/>
       <c r="T55" t="inlineStr"/>
       <c r="U55" t="inlineStr"/>
+      <c r="V55" t="inlineStr"/>
+      <c r="W55" t="inlineStr"/>
     </row>
     <row r="56">
-      <c r="A56" s="4" t="n">
+      <c r="A56" s="3" t="n">
         <v>54</v>
       </c>
       <c r="B56" t="inlineStr"/>
@@ -5598,9 +5844,11 @@
       <c r="S56" t="inlineStr"/>
       <c r="T56" t="inlineStr"/>
       <c r="U56" t="inlineStr"/>
+      <c r="V56" t="inlineStr"/>
+      <c r="W56" t="inlineStr"/>
     </row>
     <row r="57">
-      <c r="A57" s="4" t="n">
+      <c r="A57" s="3" t="n">
         <v>55</v>
       </c>
       <c r="B57" t="inlineStr"/>
@@ -5631,9 +5879,11 @@
       <c r="S57" t="inlineStr"/>
       <c r="T57" t="inlineStr"/>
       <c r="U57" t="inlineStr"/>
+      <c r="V57" t="inlineStr"/>
+      <c r="W57" t="inlineStr"/>
     </row>
     <row r="58">
-      <c r="A58" s="4" t="n">
+      <c r="A58" s="3" t="n">
         <v>56</v>
       </c>
       <c r="B58" t="inlineStr"/>
@@ -5664,9 +5914,11 @@
       <c r="S58" t="inlineStr"/>
       <c r="T58" t="inlineStr"/>
       <c r="U58" t="inlineStr"/>
+      <c r="V58" t="inlineStr"/>
+      <c r="W58" t="inlineStr"/>
     </row>
     <row r="59">
-      <c r="A59" s="4" t="n">
+      <c r="A59" s="3" t="n">
         <v>57</v>
       </c>
       <c r="B59" t="inlineStr"/>
@@ -5693,9 +5945,11 @@
       <c r="S59" t="inlineStr"/>
       <c r="T59" t="inlineStr"/>
       <c r="U59" t="inlineStr"/>
+      <c r="V59" t="inlineStr"/>
+      <c r="W59" t="inlineStr"/>
     </row>
     <row r="60">
-      <c r="A60" s="4" t="n">
+      <c r="A60" s="3" t="n">
         <v>58</v>
       </c>
       <c r="B60" t="inlineStr"/>
@@ -5722,9 +5976,11 @@
       <c r="S60" t="inlineStr"/>
       <c r="T60" t="inlineStr"/>
       <c r="U60" t="inlineStr"/>
+      <c r="V60" t="inlineStr"/>
+      <c r="W60" t="inlineStr"/>
     </row>
     <row r="61">
-      <c r="A61" s="4" t="n">
+      <c r="A61" s="3" t="n">
         <v>59</v>
       </c>
       <c r="B61" t="inlineStr"/>
@@ -5751,6 +6007,8 @@
       <c r="S61" t="inlineStr"/>
       <c r="T61" t="inlineStr"/>
       <c r="U61" t="inlineStr"/>
+      <c r="V61" t="inlineStr"/>
+      <c r="W61" t="inlineStr"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>